<commit_message>
Update all the project
</commit_message>
<xml_diff>
--- a/Documents/Project_3_Cheat_Sheet.xlsx
+++ b/Documents/Project_3_Cheat_Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Self-Learning\Columbia Fintech BootsCamp\Online Modules\Project_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Self-Learning\Columbia Fintech BootsCamp\Online Modules\Project_3\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4785F13B-52E7-4D8B-8824-8E43C6B17FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4F66BE-48CE-4C25-A058-4DC27B1FD277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8730" yWindow="345" windowWidth="20040" windowHeight="14430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6915" yWindow="1740" windowWidth="20040" windowHeight="14430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -88,9 +88,6 @@
     <t>IYW</t>
   </si>
   <si>
-    <t>Recover</t>
-  </si>
-  <si>
     <t>Utility</t>
   </si>
   <si>
@@ -146,6 +143,9 @@
   </si>
   <si>
     <t>Healthcare</t>
+  </si>
+  <si>
+    <t>Recovery</t>
   </si>
 </sst>
 </file>
@@ -244,24 +244,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,7 +562,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -569,57 +575,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="12">
+        <v>0</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="16" t="s">
+      <c r="D2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="12"/>
+      <c r="B3" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="E3" s="19" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>5</v>
@@ -629,66 +640,70 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="C4" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="G5" s="16" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="G5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="21" t="s">
         <v>2</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -699,246 +714,267 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="12">
+        <v>1</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C10" s="4"/>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3"/>
+      <c r="G11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="12">
+        <v>2</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="20" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="E14" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="12" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="2" t="s">
+      <c r="B16" s="10"/>
+      <c r="C16" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="12">
+        <v>3</v>
+      </c>
+      <c r="B17" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="8"/>
+      <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="4" t="s">
+      <c r="A18" s="12"/>
+      <c r="B18" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="7"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="4" t="s">
+      <c r="A19" s="12"/>
+      <c r="B19" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D27" s="22"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="2"/>
+      <c r="D28" s="9"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="6"/>
+      <c r="D29" s="8"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="7"/>
+      <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
-      <c r="D31" s="7"/>
+      <c r="D31" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>